<commit_message>
Adding tests for tasks, `client_review` form modified to change the name of inputs coming from task: <is_referral_for_care_ctx/>, <is_no_contact_ctx/> (was showing warning in test-harness)
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-6\zazic-scale-up\forms\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D4F694-CAD3-4049-8C8C-859D21695569}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgXdbNSGujgvtitTGOR/Ecl8pXl+w=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -396,86 +405,96 @@
   </si>
   <si>
     <t>Any Additional Comments</t>
+  </si>
+  <si>
+    <t>is_referral_for_care_ctx</t>
+  </si>
+  <si>
+    <t>is_no_contact_ctx</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="14">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF843C0B"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF548135"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <i/>
-      <sz val="11.0"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -483,7 +502,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -493,7 +512,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
@@ -507,178 +532,139 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
-    </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -868,33 +854,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.33"/>
-    <col customWidth="1" min="2" max="2" width="19.11"/>
-    <col customWidth="1" min="3" max="3" width="44.44"/>
-    <col customWidth="1" min="4" max="4" width="37.22"/>
-    <col customWidth="1" min="5" max="5" width="9.33"/>
-    <col customWidth="1" min="6" max="7" width="11.44"/>
-    <col customWidth="1" min="8" max="8" width="34.0"/>
-    <col customWidth="1" min="9" max="26" width="11.44"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="37.25" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="6" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +930,7 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="13" t="s">
         <v>42</v>
       </c>
@@ -967,7 +953,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="13" t="s">
         <v>50</v>
       </c>
@@ -990,7 +976,7 @@
       </c>
       <c r="K3" s="15"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="15.75">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -1011,12 +997,12 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75">
       <c r="A5" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>58</v>
@@ -1032,12 +1018,12 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75">
       <c r="A6" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>60</v>
@@ -1053,7 +1039,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="13" t="s">
         <v>42</v>
       </c>
@@ -1072,7 +1058,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75">
       <c r="A8" s="13" t="s">
         <v>63</v>
       </c>
@@ -1095,7 +1081,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="13" t="s">
         <v>50</v>
       </c>
@@ -1114,7 +1100,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="13" t="s">
         <v>50</v>
       </c>
@@ -1133,7 +1119,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75">
       <c r="A11" s="13" t="s">
         <v>71</v>
       </c>
@@ -1148,7 +1134,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
@@ -1163,7 +1149,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75">
       <c r="A13" s="24" t="s">
         <v>72</v>
       </c>
@@ -1199,7 +1185,7 @@
       <c r="Y13" s="25"/>
       <c r="Z13" s="25"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75">
       <c r="A14" s="26" t="s">
         <v>72</v>
       </c>
@@ -1237,7 +1223,7 @@
       <c r="Y14" s="25"/>
       <c r="Z14" s="25"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="15.75">
       <c r="A15" s="7" t="s">
         <v>72</v>
       </c>
@@ -1273,7 +1259,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75">
       <c r="A16" s="28" t="s">
         <v>72</v>
       </c>
@@ -1307,7 +1293,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75">
       <c r="A17" s="28" t="s">
         <v>72</v>
       </c>
@@ -1341,118 +1327,122 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75">
       <c r="A18" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31" t="s">
+      <c r="C18" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31"/>
-    </row>
-    <row r="19">
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75">
       <c r="A19" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31" t="s">
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="31"/>
-      <c r="Z19" s="31"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="33" t="s">
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="30"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75">
+      <c r="A20" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="34" t="s">
+      <c r="C20" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="31"/>
-    </row>
-    <row r="21">
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="30"/>
+      <c r="Y20" s="30"/>
+      <c r="Z20" s="30"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75">
       <c r="A21" s="21" t="s">
         <v>88</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="31" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="21"/>
@@ -1460,10 +1450,10 @@
       <c r="F21" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="34" t="s">
         <v>92</v>
       </c>
       <c r="I21" s="29"/>
@@ -1485,14 +1475,14 @@
       <c r="Y21" s="29"/>
       <c r="Z21" s="29"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" ht="15.75">
       <c r="A22" s="21" t="s">
         <v>93</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="21"/>
@@ -1500,7 +1490,7 @@
       <c r="F22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="35" t="s">
         <v>96</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -1525,14 +1515,14 @@
       <c r="Y22" s="29"/>
       <c r="Z22" s="29"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" ht="15.75">
       <c r="A23" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="31" t="s">
         <v>99</v>
       </c>
       <c r="D23" s="29"/>
@@ -1561,151 +1551,153 @@
       <c r="Y23" s="29"/>
       <c r="Z23" s="29"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="15.75">
       <c r="A24" s="21" t="s">
         <v>100</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31" t="s">
+      <c r="E24" s="30"/>
+      <c r="F24" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
-    </row>
-    <row r="25">
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75">
       <c r="A25" s="21" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>105</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="34" t="s">
+      <c r="E25" s="30"/>
+      <c r="F25" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="H25" s="38" t="s">
+      <c r="H25" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="31"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="31"/>
-      <c r="Z25" s="31"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="33" t="s">
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="30"/>
+      <c r="Z25" s="30"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75">
+      <c r="A26" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="21"/>
-      <c r="C26" s="32"/>
+      <c r="C26" s="31"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="33" t="s">
+      <c r="E26" s="30"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="30"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75">
+      <c r="A27" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="46" t="s">
+        <v>128</v>
+      </c>
       <c r="D27" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="31"/>
-      <c r="Y27" s="31"/>
-      <c r="Z27" s="31"/>
-    </row>
-    <row r="28">
+      <c r="E27" s="30"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75">
       <c r="A28" s="21" t="s">
         <v>83</v>
       </c>
@@ -1716,368 +1708,368 @@
         <v>111</v>
       </c>
       <c r="D28" s="29"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="34" t="s">
+      <c r="E28" s="30"/>
+      <c r="F28" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="31"/>
-      <c r="Z28" s="31"/>
-    </row>
-    <row r="29">
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="30"/>
+      <c r="Y28" s="30"/>
+      <c r="Z28" s="30"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75">
       <c r="A29" s="21" t="s">
         <v>88</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="38" t="s">
         <v>113</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="34" t="s">
+      <c r="E29" s="30"/>
+      <c r="F29" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
-      <c r="U29" s="31"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="31"/>
-      <c r="X29" s="31"/>
-      <c r="Y29" s="31"/>
-      <c r="Z29" s="31"/>
-    </row>
-    <row r="30">
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="30"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75">
       <c r="A30" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="39" t="s">
         <v>116</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="34" t="s">
+      <c r="E30" s="30"/>
+      <c r="F30" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
-      <c r="Z30" s="31"/>
-    </row>
-    <row r="31">
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="30"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="30"/>
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75">
       <c r="A31" s="21" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="36" t="s">
         <v>120</v>
       </c>
       <c r="D31" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="31"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="31"/>
-      <c r="Z31" s="31"/>
-    </row>
-    <row r="32">
+      <c r="E31" s="30"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="30"/>
+      <c r="W31" s="30"/>
+      <c r="X31" s="30"/>
+      <c r="Y31" s="30"/>
+      <c r="Z31" s="30"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75">
       <c r="A32" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="40" t="s">
         <v>99</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="34" t="s">
+      <c r="E32" s="30"/>
+      <c r="F32" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="31"/>
-      <c r="U32" s="31"/>
-      <c r="V32" s="31"/>
-      <c r="W32" s="31"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="31"/>
-      <c r="Z32" s="31"/>
-    </row>
-    <row r="33">
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="30"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75">
       <c r="A33" s="21" t="s">
         <v>100</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="34" t="s">
+      <c r="E33" s="30"/>
+      <c r="F33" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="31"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="31"/>
-      <c r="U33" s="31"/>
-      <c r="V33" s="31"/>
-      <c r="W33" s="31"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="31"/>
-      <c r="Z33" s="31"/>
-    </row>
-    <row r="34">
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="30"/>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="30"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75">
       <c r="A34" s="21" t="s">
         <v>88</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="38" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="34" t="s">
+      <c r="E34" s="30"/>
+      <c r="F34" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="38" t="s">
+      <c r="G34" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="H34" s="38" t="s">
+      <c r="H34" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="31"/>
-      <c r="R34" s="31"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="31"/>
-      <c r="U34" s="31"/>
-      <c r="V34" s="31"/>
-      <c r="W34" s="31"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="31"/>
-      <c r="Z34" s="31"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="33" t="s">
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+      <c r="Y34" s="30"/>
+      <c r="Z34" s="30"/>
+    </row>
+    <row r="35" spans="1:26" ht="15.75">
+      <c r="A35" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B35" s="21"/>
-      <c r="C35" s="42"/>
+      <c r="C35" s="41"/>
       <c r="D35" s="21"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
-      <c r="Q35" s="31"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="31"/>
-      <c r="T35" s="31"/>
-      <c r="U35" s="31"/>
-      <c r="V35" s="31"/>
-      <c r="W35" s="31"/>
-      <c r="X35" s="31"/>
-      <c r="Y35" s="31"/>
-      <c r="Z35" s="31"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="43" t="s">
+      <c r="E35" s="30"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="30"/>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="34" t="s">
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
-      <c r="Q36" s="31"/>
-      <c r="R36" s="31"/>
-      <c r="S36" s="31"/>
-      <c r="T36" s="31"/>
-      <c r="U36" s="31"/>
-      <c r="V36" s="31"/>
-      <c r="W36" s="31"/>
-      <c r="X36" s="31"/>
-      <c r="Y36" s="31"/>
-      <c r="Z36" s="31"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="34" t="s">
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="30"/>
+      <c r="Z36" s="30"/>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A37" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="34" t="s">
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
-      <c r="W37" s="46"/>
-      <c r="X37" s="46"/>
-      <c r="Y37" s="46"/>
-      <c r="Z37" s="46"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="13" t="s">
         <v>71</v>
       </c>
@@ -2092,16 +2084,16 @@
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3067,34 +3059,30 @@
     <row r="1011" ht="15.75" customHeight="1"/>
     <row r="1012" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.44"/>
-    <col customWidth="1" min="2" max="2" width="11.44"/>
-    <col customWidth="1" min="3" max="3" width="17.78"/>
-    <col customWidth="1" min="4" max="6" width="11.44"/>
-    <col customWidth="1" min="7" max="26" width="8.56"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3105,7 +3093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3116,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3127,17 +3115,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -3148,7 +3136,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -3159,7 +3147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3170,7 +3158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -3181,12 +3169,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -3197,7 +3185,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3208,93 +3196,93 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4257,32 +4245,28 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.89"/>
-    <col customWidth="1" min="2" max="2" width="43.67"/>
-    <col customWidth="1" min="3" max="3" width="32.89"/>
-    <col customWidth="1" min="4" max="4" width="20.89"/>
-    <col customWidth="1" min="5" max="15" width="11.44"/>
-    <col customWidth="1" min="16" max="26" width="8.78"/>
+    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="3" max="3" width="32.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="26" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
+    <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4328,7 +4312,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>39</v>
       </c>
@@ -4336,7 +4320,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="11">
-        <v>43894.0</v>
+        <v>43894</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>41</v>
@@ -5353,9 +5337,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zazic-scale-up: #35 partner feedback
- https://github.com/medic/config-itech/issues/35#issuecomment-646054424
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -1,49 +1,403 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-6\zazic-scale-up\forms\app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D4F694-CAD3-4049-8C8C-859D21695569}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgXdbNSGujgvtitTGOR/Ecl8pXl+w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mi9WHKUeL+WS2J7XfkOcLJP6DzYhA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
   <si>
     <t>type</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>is_referral_for_care_ctx</t>
+  </si>
+  <si>
+    <t>Is a referral for care case</t>
+  </si>
+  <si>
+    <t>is_no_contact_ctx</t>
+  </si>
+  <si>
+    <t>Is a no contact case</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:person</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Select a person from list</t>
+  </si>
+  <si>
+    <t>Patient Name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>patient_name</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>Patient Phone</t>
+  </si>
+  <si>
+    <t>../inputs/contact/phone</t>
+  </si>
+  <si>
+    <t>is_referral_for_care</t>
+  </si>
+  <si>
+    <t>../inputs/is_referral_for_care</t>
+  </si>
+  <si>
+    <t>is_no_contact</t>
+  </si>
+  <si>
+    <t>../inputs/is_no_contact</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>select_one yes_no</t>
+  </si>
+  <si>
+    <t>client_came</t>
+  </si>
+  <si>
+    <t>Did client return to clinic?</t>
+  </si>
+  <si>
+    <t>return_client</t>
+  </si>
+  <si>
+    <t>${client_came} = 'yes'</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>clinic_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which clinic? </t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
+  </si>
+  <si>
+    <t>Please type in name characters e.g letters and space.</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>visit_date</t>
+  </si>
+  <si>
+    <t>Date of visit/review</t>
+  </si>
+  <si>
+    <t>. &lt;= today() and ((decimal-date-time(today()) - decimal-date-time(.)) &lt;= 28)</t>
+  </si>
+  <si>
+    <t>Visit date must be within the past 4 weeks</t>
+  </si>
+  <si>
+    <t>ae_positive</t>
+  </si>
+  <si>
+    <t>Did nurse identify an AE?</t>
+  </si>
+  <si>
+    <t>select_one severities</t>
+  </si>
+  <si>
+    <t>ae_severity</t>
+  </si>
+  <si>
+    <t>Severity of the Adverse Event (AE)</t>
+  </si>
+  <si>
+    <t>../ae_positive = 'yes'</t>
+  </si>
+  <si>
+    <t>ae_type</t>
+  </si>
+  <si>
+    <t>AE Code</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\-]+$")</t>
+  </si>
+  <si>
+    <t>Please type in proper characters e.g AN-A</t>
+  </si>
+  <si>
+    <t>trace_client</t>
+  </si>
+  <si>
+    <t>${client_came}='no'</t>
+  </si>
+  <si>
+    <t>client_traced</t>
+  </si>
+  <si>
+    <t>Have you traced the client?</t>
+  </si>
+  <si>
+    <t>client_not_traced_reason</t>
+  </si>
+  <si>
+    <t>If no tracing, explain why not.</t>
+  </si>
+  <si>
+    <t>${client_traced} = 'no'</t>
+  </si>
+  <si>
+    <t>select_one tracing_methods</t>
+  </si>
+  <si>
+    <t>tracing_method</t>
+  </si>
+  <si>
+    <t>How did you trace the client</t>
+  </si>
+  <si>
+    <t>${client_traced} = 'yes'</t>
+  </si>
+  <si>
+    <t>client_ok</t>
+  </si>
+  <si>
+    <t>Is VMMC Client okay?</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>n_thanks</t>
+  </si>
+  <si>
+    <t>Thanks for tracing the client</t>
+  </si>
+  <si>
+    <t>q_ae_positive</t>
+  </si>
+  <si>
+    <t>if(${tracing_method} = "phone", "Did nurse suspect an AE?", "Did nurse identify an AE?")</t>
+  </si>
+  <si>
+    <t>${q_ae_positive}</t>
+  </si>
+  <si>
+    <t>${client_ok} = 'no'</t>
+  </si>
+  <si>
+    <t>additional_comments</t>
+  </si>
+  <si>
+    <t>Any Additional Comments</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>Name of health provider/Nurse</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
+    <t>action_types</t>
+  </si>
+  <si>
+    <t>no_response</t>
+  </si>
+  <si>
+    <t>Report a No response by day 7</t>
+  </si>
+  <si>
+    <t>report_ae</t>
+  </si>
+  <si>
+    <t>Report an AE</t>
+  </si>
+  <si>
+    <t>severities</t>
+  </si>
+  <si>
+    <t>mild</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>severe</t>
+  </si>
+  <si>
+    <t>Severe</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>tracing_methods</t>
+  </si>
+  <si>
+    <t>By phone</t>
+  </si>
+  <si>
+    <t>in_person</t>
+  </si>
+  <si>
+    <t>In person</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>form_id</t>
   </si>
   <si>
@@ -53,99 +407,18 @@
     <t>style</t>
   </si>
   <si>
-    <t>action_types</t>
-  </si>
-  <si>
-    <t>no_response</t>
-  </si>
-  <si>
-    <t>Report a No response by day 7</t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
-    <t>report_ae</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>Report an AE</t>
-  </si>
-  <si>
     <t>instance_name</t>
   </si>
   <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
     <t>formId</t>
   </si>
   <si>
     <t>default_language</t>
   </si>
   <si>
-    <t>severities</t>
-  </si>
-  <si>
-    <t>mild</t>
-  </si>
-  <si>
-    <t>Mild</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>severe</t>
-  </si>
-  <si>
-    <t>Severe</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Client Review</t>
   </si>
   <si>
@@ -155,9 +428,6 @@
     <t>pages</t>
   </si>
   <si>
-    <t>begin group</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -165,344 +435,95 @@
   </si>
   <si>
     <t>en</t>
-  </si>
-  <si>
-    <t>inputs</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>./source = 'user'</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>hidden</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>source_id</t>
-  </si>
-  <si>
-    <t>Source ID</t>
-  </si>
-  <si>
-    <t>is_referral_for_care</t>
-  </si>
-  <si>
-    <t>Is a referral for care case</t>
-  </si>
-  <si>
-    <t>is_no_contact</t>
-  </si>
-  <si>
-    <t>Is a no contact case</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>db:person</t>
-  </si>
-  <si>
-    <t>_id</t>
-  </si>
-  <si>
-    <t>What is the patient's name?</t>
-  </si>
-  <si>
-    <t>db-object</t>
-  </si>
-  <si>
-    <t>Select a person from list</t>
-  </si>
-  <si>
-    <t>Patient Name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>end group</t>
-  </si>
-  <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>patient_name</t>
-  </si>
-  <si>
-    <t>../inputs/contact/name</t>
-  </si>
-  <si>
-    <t>patient_id</t>
-  </si>
-  <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
-    <t>../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t>Patient Phone</t>
-  </si>
-  <si>
-    <t>../inputs/contact/phone</t>
-  </si>
-  <si>
-    <t>../inputs/is_referral_for_care</t>
-  </si>
-  <si>
-    <t>../inputs/is_no_contact</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>select_one yes_no</t>
-  </si>
-  <si>
-    <t>client_came</t>
-  </si>
-  <si>
-    <t>Did client return to clinic?</t>
-  </si>
-  <si>
-    <t>return_client</t>
-  </si>
-  <si>
-    <t>${client_came} = 'yes'</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>clinic_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which clinic? </t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
-  </si>
-  <si>
-    <t>Please type in name characters e.g letters and space.</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>visit_date</t>
-  </si>
-  <si>
-    <t>Date of visit/review</t>
-  </si>
-  <si>
-    <t>. &lt;= today() and ((decimal-date-time(today()) - decimal-date-time(.)) &lt;= 28)</t>
-  </si>
-  <si>
-    <t>Visit date must be within the past 4 weeks</t>
-  </si>
-  <si>
-    <t>ae_positive</t>
-  </si>
-  <si>
-    <t>Did nurse identify an AE?</t>
-  </si>
-  <si>
-    <t>select_one severities</t>
-  </si>
-  <si>
-    <t>ae_severity</t>
-  </si>
-  <si>
-    <t>Severity of the Adverse Event (AE)</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes'</t>
-  </si>
-  <si>
-    <t>ae_type</t>
-  </si>
-  <si>
-    <t>AE type and timing</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\-]+$")</t>
-  </si>
-  <si>
-    <t>Please type in proper characters e.g AN-A</t>
-  </si>
-  <si>
-    <t>trace_client</t>
-  </si>
-  <si>
-    <t>${client_came}='no'</t>
-  </si>
-  <si>
-    <t>client_traced</t>
-  </si>
-  <si>
-    <t>Have you traced the client?</t>
-  </si>
-  <si>
-    <t>client_not_traced_reason</t>
-  </si>
-  <si>
-    <t>No tracing, explain why not.</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'no'</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'yes'</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>n_thanks</t>
-  </si>
-  <si>
-    <t>Thanks for tracing the client</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'no'</t>
-  </si>
-  <si>
-    <t>nurse</t>
-  </si>
-  <si>
-    <t>Name of health provider/Nurse</t>
-  </si>
-  <si>
-    <t>additional_comments</t>
-  </si>
-  <si>
-    <t>Any Additional Comments</t>
-  </si>
-  <si>
-    <t>is_referral_for_care_ctx</t>
-  </si>
-  <si>
-    <t>is_no_contact_ctx</t>
-  </si>
-  <si>
-    <t>NO_LABEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="14">
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Proxima Nova"/>
+      <sz val="11.0"/>
+      <color rgb="FF843C0B"/>
+      <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <color rgb="FF833C0C"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF548135"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Cambria"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Proxima Nova"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF843C0B"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF833C0C"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF548135"/>
-      <name val="Cambria"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -510,14 +531,20 @@
         <bgColor rgb="FF2E75B6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
+    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -532,139 +559,110 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="47">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+  <cellXfs count="32">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="2" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -854,310 +852,314 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1012"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="44.5" customWidth="1"/>
-    <col min="4" max="4" width="37.25" customWidth="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1"/>
-    <col min="6" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="34" customWidth="1"/>
-    <col min="9" max="26" width="11.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="20.33"/>
+    <col customWidth="1" min="2" max="2" width="19.11"/>
+    <col customWidth="1" min="3" max="3" width="44.44"/>
+    <col customWidth="1" min="4" max="4" width="37.22"/>
+    <col customWidth="1" min="5" max="5" width="9.33"/>
+    <col customWidth="1" min="6" max="7" width="11.44"/>
+    <col customWidth="1" min="8" max="8" width="34.0"/>
+    <col customWidth="1" min="9" max="26" width="11.44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75">
-      <c r="A2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75">
-      <c r="A3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75">
-      <c r="A4" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75">
-      <c r="A5" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75">
-      <c r="A6" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75">
-      <c r="A7" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75">
-      <c r="A8" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75">
-      <c r="A9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75">
-      <c r="A10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75">
-      <c r="A11" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12">
       <c r="A12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75">
-      <c r="A13" s="24" t="s">
-        <v>72</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>68</v>
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1167,81 +1169,81 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75">
-      <c r="A14" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75">
-      <c r="A15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7" t="s">
-        <v>79</v>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1259,14 +1261,14 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75">
-      <c r="A16" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="3"/>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1274,8 +1276,8 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="28" t="s">
-        <v>80</v>
+      <c r="K16" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1293,14 +1295,14 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75">
-      <c r="A17" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="3"/>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1308,8 +1310,8 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="28" t="s">
-        <v>81</v>
+      <c r="K17" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1327,773 +1329,845 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75">
-      <c r="A18" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="29" t="s">
+    <row r="18">
+      <c r="A18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.75">
-      <c r="A19" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="D29" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="E29" s="8"/>
+      <c r="F29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="30"/>
-      <c r="Z19" s="30"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.75">
-      <c r="A20" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="21" t="s">
+      <c r="B30" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" s="33" t="s">
+      <c r="C30" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="30"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="30"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75">
-      <c r="A21" s="21" t="s">
+      <c r="D30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="E30" s="8"/>
+      <c r="F30" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C31" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="34" t="s">
+      <c r="D31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="B32" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-      <c r="W21" s="29"/>
-      <c r="X21" s="29"/>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75">
-      <c r="A22" s="21" t="s">
+      <c r="C32" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="D32" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C33" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="35" t="s">
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="D34" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="29"/>
-    </row>
-    <row r="23" spans="1:26" ht="15.75">
-      <c r="A23" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="E34" s="8"/>
+      <c r="F34" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C38" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
-      <c r="X23" s="29"/>
-      <c r="Y23" s="29"/>
-      <c r="Z23" s="29"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75">
-      <c r="A24" s="21" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C39" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75">
-      <c r="A25" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-    </row>
-    <row r="26" spans="1:26" ht="15.75">
-      <c r="A26" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75">
-      <c r="A27" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75">
-      <c r="A28" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75">
-      <c r="A29" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75">
-      <c r="A30" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75">
-      <c r="A31" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="30"/>
-    </row>
-    <row r="32" spans="1:26" ht="15.75">
-      <c r="A32" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75">
-      <c r="A33" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="30"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="30"/>
-      <c r="Z33" s="30"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75">
-      <c r="A34" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="H34" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
-    </row>
-    <row r="35" spans="1:26" ht="15.75">
-      <c r="A35" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-    </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="30"/>
-      <c r="Z36" s="30"/>
-    </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="33" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-    </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-    </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3058,231 +3132,249 @@
     <row r="1010" ht="15.75" customHeight="1"/>
     <row r="1011" ht="15.75" customHeight="1"/>
     <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C993"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
-    <col min="4" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="26" width="8.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="16.44"/>
+    <col customWidth="1" min="2" max="2" width="11.44"/>
+    <col customWidth="1" min="3" max="3" width="17.78"/>
+    <col customWidth="1" min="4" max="6" width="11.44"/>
+    <col customWidth="1" min="7" max="26" width="8.44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1">
       <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
+      <c r="C4" s="26"/>
+    </row>
+    <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C14" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
+      <c r="C31" s="26"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4245,116 +4337,120 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.875" customWidth="1"/>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="15" width="11.5" customWidth="1"/>
-    <col min="16" max="26" width="8.75" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="31.89"/>
+    <col customWidth="1" min="2" max="2" width="43.67"/>
+    <col customWidth="1" min="3" max="3" width="32.89"/>
+    <col customWidth="1" min="4" max="4" width="20.89"/>
+    <col customWidth="1" min="5" max="15" width="11.44"/>
+    <col customWidth="1" min="16" max="26" width="8.78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="11">
-        <v>43894</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
+    <row r="1" ht="18.0" customHeight="1">
+      <c r="A1" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="31">
+        <v>43894.0</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -5337,7 +5433,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zazic-scale-up: #35 make patient name required
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
   <si>
     <t>type</t>
   </si>
@@ -119,6 +119,9 @@
     <t>db-object</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>Select a person from list</t>
   </si>
   <si>
@@ -147,9 +150,6 @@
   </si>
   <si>
     <t>Patient ID</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>../inputs/contact/_id</t>
@@ -589,13 +589,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1070,11 +1070,13 @@
       <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1083,14 +1085,14 @@
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="1"/>
@@ -1104,14 +1106,14 @@
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>35</v>
+      <c r="B10" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="1"/>
@@ -1123,12 +1125,12 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="9"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1138,9 +1140,9 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="10"/>
+        <v>38</v>
+      </c>
+      <c r="B12" s="11"/>
       <c r="C12" s="9"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1153,13 +1155,13 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1169,7 +1171,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -1189,21 +1191,21 @@
     </row>
     <row r="14">
       <c r="A14" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+        <v>33</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="15" t="s">
@@ -1227,10 +1229,10 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>45</v>
@@ -1263,7 +1265,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>47</v>
@@ -1297,7 +1299,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>49</v>
@@ -1378,7 +1380,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -1450,7 +1452,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>61</v>
@@ -1490,7 +1492,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>66</v>
@@ -1530,7 +1532,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -1568,7 +1570,7 @@
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -1606,7 +1608,7 @@
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>76</v>
@@ -1635,7 +1637,7 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="17"/>
@@ -1712,7 +1714,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -1750,7 +1752,7 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -1774,10 +1776,10 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="21" t="s">
@@ -1787,8 +1789,8 @@
         <v>88</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="11" t="s">
-        <v>43</v>
+      <c r="F30" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
@@ -1826,7 +1828,7 @@
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -1886,10 +1888,10 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="11" t="s">
+      <c r="A33" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="23" t="s">
@@ -1902,7 +1904,7 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="12" t="s">
         <v>95</v>
       </c>
       <c r="L33" s="8"/>
@@ -1936,7 +1938,7 @@
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -1974,7 +1976,7 @@
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
@@ -2012,7 +2014,7 @@
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G36" s="18" t="s">
         <v>76</v>
@@ -2041,7 +2043,7 @@
     </row>
     <row r="37">
       <c r="A37" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="2"/>
@@ -2118,7 +2120,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G39" s="18" t="s">
         <v>61</v>
@@ -2147,7 +2149,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3259,7 +3261,7 @@
         <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>119</v>
@@ -3277,24 +3279,24 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>

<commit_message>
zazic-scale-up: #35 client review msc flow updates
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mi9WHKUeL+WS2J7XfkOcLJP6DzYhA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhGA2rHGT2d/E/8q1x8a36p9KSGYA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="170">
   <si>
     <t>type</t>
   </si>
@@ -194,126 +194,150 @@
     <t>${client_came} = 'yes'</t>
   </si>
   <si>
+    <t>select_one facilities</t>
+  </si>
+  <si>
+    <t>clinic_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which clinic? </t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
+  </si>
+  <si>
+    <t>Please type in name characters e.g letters and space.</t>
+  </si>
+  <si>
+    <t>clinic_name_other</t>
+  </si>
+  <si>
+    <t>Specify Other</t>
+  </si>
+  <si>
+    <t>${clinic_name} = 'other'</t>
+  </si>
+  <si>
+    <t>Please enter a valid clinic name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>visit_date</t>
+  </si>
+  <si>
+    <t>Date of visit/review</t>
+  </si>
+  <si>
+    <t>. &lt;= today() and ((decimal-date-time(today()) - decimal-date-time(.)) &lt;= 28)</t>
+  </si>
+  <si>
+    <t>Date is not in the future: and not more than 4 weeks ago</t>
+  </si>
+  <si>
+    <t>ae_positive</t>
+  </si>
+  <si>
+    <t>Did nurse identify an AE?</t>
+  </si>
+  <si>
+    <t>select_one severities</t>
+  </si>
+  <si>
+    <t>ae_severity</t>
+  </si>
+  <si>
+    <t>Severity of the Adverse Event (AE)</t>
+  </si>
+  <si>
+    <t>../ae_positive = 'yes'</t>
+  </si>
+  <si>
+    <t>ae_type</t>
+  </si>
+  <si>
+    <t>AE Code</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z\-]+$")</t>
+  </si>
+  <si>
+    <t>The AE Code should be captured in the same way they are recorded in the VMMC register</t>
+  </si>
+  <si>
+    <t>Should be the same AE Code as the one used in the register</t>
+  </si>
+  <si>
+    <t>trace_client</t>
+  </si>
+  <si>
+    <t>${client_came}='no'</t>
+  </si>
+  <si>
+    <t>select_one tracing_methods</t>
+  </si>
+  <si>
+    <t>tracing_method</t>
+  </si>
+  <si>
+    <t>Have you traced the client?</t>
+  </si>
+  <si>
+    <t>client_traced</t>
+  </si>
+  <si>
+    <t>if(${tracing_method} = 'in_person', 'yes', if(${tracing_method} = 'phone', 'yes', 'no'))</t>
+  </si>
+  <si>
+    <t>client_not_traced_reason</t>
+  </si>
+  <si>
+    <t>If no tracing, explain why not.</t>
+  </si>
+  <si>
+    <t>${client_traced} = 'no'</t>
+  </si>
+  <si>
+    <t>client_ok</t>
+  </si>
+  <si>
+    <t>Is VMMC Client okay?</t>
+  </si>
+  <si>
+    <t>${client_traced} = 'yes'</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>n_thanks</t>
+  </si>
+  <si>
+    <t>Thanks for tracing the client</t>
+  </si>
+  <si>
+    <t>${client_ok} = 'yes'</t>
+  </si>
+  <si>
+    <t>q_ae_positive</t>
+  </si>
+  <si>
+    <t>if(${tracing_method} = "in_person", "Did nurse identify an AE?", "Did nurse suspect an AE?")</t>
+  </si>
+  <si>
+    <t>${q_ae_positive}</t>
+  </si>
+  <si>
+    <t>${client_ok} = 'no'</t>
+  </si>
+  <si>
+    <t>../ae_positive = 'yes' and ${tracing_method} = 'in_person'</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
-    <t>clinic_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which clinic? </t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
-  </si>
-  <si>
-    <t>Please type in name characters e.g letters and space.</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>visit_date</t>
-  </si>
-  <si>
-    <t>Date of visit/review</t>
-  </si>
-  <si>
-    <t>. &lt;= today() and ((decimal-date-time(today()) - decimal-date-time(.)) &lt;= 28)</t>
-  </si>
-  <si>
-    <t>Visit date must be within the past 4 weeks</t>
-  </si>
-  <si>
-    <t>ae_positive</t>
-  </si>
-  <si>
-    <t>Did nurse identify an AE?</t>
-  </si>
-  <si>
-    <t>select_one severities</t>
-  </si>
-  <si>
-    <t>ae_severity</t>
-  </si>
-  <si>
-    <t>Severity of the Adverse Event (AE)</t>
-  </si>
-  <si>
-    <t>../ae_positive = 'yes'</t>
-  </si>
-  <si>
-    <t>ae_type</t>
-  </si>
-  <si>
-    <t>AE Code</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\-]+$")</t>
-  </si>
-  <si>
-    <t>Please type in proper characters e.g AN-A</t>
-  </si>
-  <si>
-    <t>trace_client</t>
-  </si>
-  <si>
-    <t>${client_came}='no'</t>
-  </si>
-  <si>
-    <t>client_traced</t>
-  </si>
-  <si>
-    <t>Have you traced the client?</t>
-  </si>
-  <si>
-    <t>client_not_traced_reason</t>
-  </si>
-  <si>
-    <t>If no tracing, explain why not.</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'no'</t>
-  </si>
-  <si>
-    <t>select_one tracing_methods</t>
-  </si>
-  <si>
-    <t>tracing_method</t>
-  </si>
-  <si>
-    <t>How did you trace the client</t>
-  </si>
-  <si>
-    <t>${client_traced} = 'yes'</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Is VMMC Client okay?</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>n_thanks</t>
-  </si>
-  <si>
-    <t>Thanks for tracing the client</t>
-  </si>
-  <si>
-    <t>q_ae_positive</t>
-  </si>
-  <si>
-    <t>if(${tracing_method} = "phone", "Did nurse suspect an AE?", "Did nurse identify an AE?")</t>
-  </si>
-  <si>
-    <t>${q_ae_positive}</t>
-  </si>
-  <si>
-    <t>${client_ok} = 'no'</t>
-  </si>
-  <si>
     <t>additional_comments</t>
   </si>
   <si>
@@ -368,31 +392,103 @@
     <t>Severe</t>
   </si>
   <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>tracing_methods</t>
+  </si>
+  <si>
+    <t>in_person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Yes, Via Physical visit
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Yes, Via Phone call
+</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>3. No</t>
+  </si>
+  <si>
+    <t>facilities</t>
+  </si>
+  <si>
+    <t>seke_north</t>
+  </si>
+  <si>
+    <t>1. Chitungwiza-Seke North clinic</t>
+  </si>
+  <si>
+    <t>seke_south</t>
+  </si>
+  <si>
+    <t>2. Chitungwiza-Seke South clinic</t>
+  </si>
+  <si>
+    <t>city_med</t>
+  </si>
+  <si>
+    <t>3. Chitungwiza-City Med hospital</t>
+  </si>
+  <si>
+    <t>zengeza</t>
+  </si>
+  <si>
+    <t>4. Chitungwiza-Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>chitungwiza_central</t>
+  </si>
+  <si>
+    <t>5. Chitungwiza-Chitungwiza Central Hospital</t>
+  </si>
+  <si>
+    <t>chegutu_norton</t>
+  </si>
+  <si>
+    <t>6. Chegutu- Norton hospital</t>
+  </si>
+  <si>
+    <t>chegutu_district</t>
+  </si>
+  <si>
+    <t>7. Chegutu- District Hospital</t>
+  </si>
+  <si>
+    <t>monera</t>
+  </si>
+  <si>
+    <t>8. Chegutu- Monera clinic (Norton Outreach)</t>
+  </si>
+  <si>
+    <t>marondera</t>
+  </si>
+  <si>
+    <t>9. Marondera- Marondera District Hospital</t>
+  </si>
+  <si>
+    <t>mahusekwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Marondera- Mahusekwa Hospital
+</t>
+  </si>
+  <si>
     <t>other</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>tracing_methods</t>
-  </si>
-  <si>
-    <t>By phone</t>
-  </si>
-  <si>
-    <t>in_person</t>
-  </si>
-  <si>
-    <t>In person</t>
+    <t>11. Other</t>
   </si>
   <si>
     <t>form_title</t>
@@ -444,7 +540,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -487,6 +583,10 @@
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -564,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -613,11 +713,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -625,20 +728,26 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -873,7 +982,8 @@
     <col customWidth="1" min="3" max="3" width="44.44"/>
     <col customWidth="1" min="4" max="4" width="37.22"/>
     <col customWidth="1" min="5" max="5" width="9.33"/>
-    <col customWidth="1" min="6" max="7" width="11.44"/>
+    <col customWidth="1" min="6" max="6" width="11.44"/>
+    <col customWidth="1" min="7" max="7" width="52.33"/>
     <col customWidth="1" min="8" max="8" width="34.0"/>
     <col customWidth="1" min="9" max="26" width="11.44"/>
   </cols>
@@ -1440,7 +1550,7 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1480,25 +1590,27 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="D22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1521,7 +1633,7 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>68</v>
@@ -1534,8 +1646,12 @@
       <c r="F23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1557,17 +1673,15 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
         <v>33</v>
@@ -1595,27 +1709,23 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="19" t="s">
         <v>75</v>
       </c>
+      <c r="C25" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="D25" s="8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1636,17 +1746,31 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="8"/>
+      <c r="A26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="F26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -1667,17 +1791,11 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>79</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1702,20 +1820,20 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="s">
-        <v>53</v>
+      <c r="A28" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -1738,20 +1856,18 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="A29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="8"/>
@@ -1777,26 +1893,26 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>88</v>
       </c>
+      <c r="C30" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="8" t="s">
         <v>33</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
@@ -1814,17 +1930,17 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31">
-      <c r="A31" s="8" t="s">
-        <v>53</v>
+      <c r="A31" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
@@ -1851,21 +1967,13 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32">
-      <c r="A32" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>88</v>
-      </c>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1888,25 +1996,27 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="8"/>
+      <c r="D33" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="F33" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
-      <c r="K33" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -1925,24 +2035,22 @@
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="8" t="s">
         <v>97</v>
       </c>
+      <c r="C34" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -1962,27 +2070,25 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35">
-      <c r="A35" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="A35" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="K35" s="12" t="s">
+        <v>101</v>
+      </c>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -2001,27 +2107,23 @@
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2042,14 +2144,22 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37">
-      <c r="A37" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="8"/>
+      <c r="A37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="F37" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -2071,24 +2181,32 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38">
       <c r="A38" s="8" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -2107,27 +2225,17 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>102</v>
-      </c>
+    <row r="39">
+      <c r="A39" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -2148,22 +2256,96 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
     <row r="43" ht="15.75" customHeight="1"/>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1"/>
@@ -3136,6 +3318,8 @@
     <row r="1012" ht="15.75" customHeight="1"/>
     <row r="1013" ht="15.75" customHeight="1"/>
     <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
@@ -3159,14 +3343,14 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="16.44"/>
     <col customWidth="1" min="2" max="2" width="11.44"/>
-    <col customWidth="1" min="3" max="3" width="17.78"/>
+    <col customWidth="1" min="3" max="3" width="31.22"/>
     <col customWidth="1" min="4" max="6" width="11.44"/>
     <col customWidth="1" min="7" max="26" width="8.44"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3177,30 +3361,30 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="26"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
@@ -3209,95 +3393,95 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -3306,75 +3490,141 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="A18" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1"/>
+    <row r="29">
+      <c r="A29" s="12"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1"/>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="12"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="26"/>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
@@ -4365,94 +4615,94 @@
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="A1" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
+      <c r="H1" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="31">
+      <c r="A2" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="34">
         <v>43894.0</v>
       </c>
-      <c r="D2" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
+      <c r="D2" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Removing validation from a select field #90
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-master\zazic-scale-up\forms\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6173F5-28E0-4217-AE17-42A69D8587BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mhGA2rHGT2d/E/8q1x8a36p9KSGYA=="/>
@@ -18,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="170">
   <si>
     <t>type</t>
   </si>
@@ -536,84 +545,84 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="15">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF843C0B"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF548135"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -623,7 +632,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -639,12 +648,19 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -659,119 +675,105 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -961,34 +963,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.33"/>
-    <col customWidth="1" min="2" max="2" width="19.11"/>
-    <col customWidth="1" min="3" max="3" width="44.44"/>
-    <col customWidth="1" min="4" max="4" width="37.22"/>
-    <col customWidth="1" min="5" max="5" width="9.33"/>
-    <col customWidth="1" min="6" max="6" width="11.44"/>
-    <col customWidth="1" min="7" max="7" width="52.33"/>
-    <col customWidth="1" min="8" max="8" width="34.0"/>
-    <col customWidth="1" min="9" max="26" width="11.44"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="37.25" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="52.375" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1040,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1061,7 +1063,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1084,7 +1086,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" ht="15.75">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1105,7 +1107,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" ht="15.75">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1126,7 +1128,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:26" ht="15.75">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1147,7 +1149,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1166,7 +1168,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1193,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1214,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1233,7 +1235,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1248,7 +1250,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1263,7 +1265,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -1299,7 +1301,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75">
       <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
@@ -1337,7 +1339,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="15.75">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1373,7 +1375,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1409,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1443,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1479,7 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:26" ht="15.75">
       <c r="A19" s="8" t="s">
         <v>53</v>
       </c>
@@ -1513,7 +1515,7 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:26" ht="15.75">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -1549,7 +1551,7 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:26" ht="15.75">
       <c r="A21" s="12" t="s">
         <v>58</v>
       </c>
@@ -1564,12 +1566,8 @@
       <c r="F21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1589,7 +1587,7 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:26" ht="15.75">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -1631,7 +1629,7 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:26" ht="15.75">
       <c r="A23" s="8" t="s">
         <v>67</v>
       </c>
@@ -1671,7 +1669,7 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:26" ht="15.75">
       <c r="A24" s="8" t="s">
         <v>53</v>
       </c>
@@ -1707,7 +1705,7 @@
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:26" ht="15.75">
       <c r="A25" s="8" t="s">
         <v>74</v>
       </c>
@@ -1745,7 +1743,7 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:26" ht="15.75">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -1789,7 +1787,7 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:26" ht="15.75">
       <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
@@ -1819,7 +1817,7 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:26" ht="15.75">
       <c r="A28" s="13" t="s">
         <v>11</v>
       </c>
@@ -1855,7 +1853,7 @@
       <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:26" ht="15.75">
       <c r="A29" s="12" t="s">
         <v>85</v>
       </c>
@@ -1891,7 +1889,7 @@
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:26" ht="15.75">
       <c r="A30" s="12" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1927,7 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:26" ht="15.75">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
@@ -1967,7 +1965,7 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="16"/>
@@ -1995,7 +1993,7 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:26" ht="15.75">
       <c r="A33" s="8" t="s">
         <v>53</v>
       </c>
@@ -2033,7 +2031,7 @@
       <c r="Y33" s="8"/>
       <c r="Z33" s="8"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:26" ht="15.75">
       <c r="A34" s="8" t="s">
         <v>96</v>
       </c>
@@ -2069,7 +2067,7 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:26" ht="15.75">
       <c r="A35" s="12" t="s">
         <v>39</v>
       </c>
@@ -2105,7 +2103,7 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:26" ht="15.75">
       <c r="A36" s="8" t="s">
         <v>53</v>
       </c>
@@ -2143,7 +2141,7 @@
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:26" ht="15.75">
       <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
@@ -2181,7 +2179,7 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:26" ht="15.75">
       <c r="A38" s="8" t="s">
         <v>105</v>
       </c>
@@ -2225,7 +2223,7 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:26" ht="15.75">
       <c r="A39" s="13" t="s">
         <v>38</v>
       </c>
@@ -2255,7 +2253,7 @@
       <c r="Y39" s="8"/>
       <c r="Z39" s="8"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>105</v>
       </c>
@@ -2291,7 +2289,7 @@
       <c r="Y40" s="8"/>
       <c r="Z40" s="8"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="26" t="s">
         <v>16</v>
       </c>
@@ -2331,7 +2329,7 @@
       <c r="Y41" s="8"/>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>38</v>
       </c>
@@ -2346,12 +2344,12 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3321,34 +3319,30 @@
     <row r="1015" ht="15.75" customHeight="1"/>
     <row r="1016" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.44"/>
-    <col customWidth="1" min="2" max="2" width="11.44"/>
-    <col customWidth="1" min="3" max="3" width="31.22"/>
-    <col customWidth="1" min="4" max="6" width="11.44"/>
-    <col customWidth="1" min="7" max="26" width="8.44"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="31.25" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -3359,7 +3353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -3370,7 +3364,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -3381,17 +3375,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>117</v>
       </c>
@@ -3402,7 +3396,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>117</v>
       </c>
@@ -3413,7 +3407,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>117</v>
       </c>
@@ -3424,12 +3418,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>124</v>
       </c>
@@ -3440,7 +3434,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>124</v>
       </c>
@@ -3451,7 +3445,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="12" t="s">
         <v>127</v>
       </c>
@@ -3462,7 +3456,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>127</v>
       </c>
@@ -3473,7 +3467,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>127</v>
       </c>
@@ -3484,12 +3478,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="28" t="s">
         <v>133</v>
       </c>
@@ -3500,7 +3494,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="28" t="s">
         <v>133</v>
       </c>
@@ -3511,7 +3505,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="28" t="s">
         <v>133</v>
       </c>
@@ -3522,7 +3516,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="28" t="s">
         <v>133</v>
       </c>
@@ -3533,7 +3527,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="28" t="s">
         <v>133</v>
       </c>
@@ -3544,7 +3538,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="28" t="s">
         <v>133</v>
       </c>
@@ -3555,7 +3549,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="28" t="s">
         <v>133</v>
       </c>
@@ -3566,7 +3560,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="28" t="s">
         <v>133</v>
       </c>
@@ -3577,7 +3571,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="28" t="s">
         <v>133</v>
       </c>
@@ -3588,7 +3582,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="28" t="s">
         <v>133</v>
       </c>
@@ -3599,7 +3593,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="28" t="s">
         <v>133</v>
       </c>
@@ -3610,23 +3604,23 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:3" ht="15.75">
       <c r="A29" s="12"/>
       <c r="B29" s="1"/>
       <c r="C29" s="12"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="12"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="1"/>
       <c r="C31" s="27"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4589,32 +4583,28 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.89"/>
-    <col customWidth="1" min="2" max="2" width="43.67"/>
-    <col customWidth="1" min="3" max="3" width="32.89"/>
-    <col customWidth="1" min="4" max="4" width="20.89"/>
-    <col customWidth="1" min="5" max="15" width="11.44"/>
-    <col customWidth="1" min="16" max="26" width="8.78"/>
+    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="3" max="3" width="32.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="26" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
+    <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>156</v>
       </c>
@@ -4660,7 +4650,7 @@
       <c r="Y1" s="31"/>
       <c r="Z1" s="31"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>164</v>
       </c>
@@ -4668,7 +4658,7 @@
         <v>165</v>
       </c>
       <c r="C2" s="34">
-        <v>43894.0</v>
+        <v>43894</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>166</v>
@@ -5685,9 +5675,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new facilities to xlsx files
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-master\zazic-scale-up\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6173F5-28E0-4217-AE17-42A69D8587BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CB4B1F-45F9-BD44-9A44-4620284A7BD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="184">
   <si>
     <t>type</t>
   </si>
@@ -448,21 +448,12 @@
     <t>city_med</t>
   </si>
   <si>
-    <t>3. Chitungwiza-City Med hospital</t>
-  </si>
-  <si>
     <t>zengeza</t>
   </si>
   <si>
-    <t>4. Chitungwiza-Zengeza Clinic</t>
-  </si>
-  <si>
     <t>chitungwiza_central</t>
   </si>
   <si>
-    <t>5. Chitungwiza-Chitungwiza Central Hospital</t>
-  </si>
-  <si>
     <t>chegutu_norton</t>
   </si>
   <si>
@@ -472,34 +463,18 @@
     <t>chegutu_district</t>
   </si>
   <si>
-    <t>7. Chegutu- District Hospital</t>
-  </si>
-  <si>
     <t>monera</t>
   </si>
   <si>
-    <t>8. Chegutu- Monera clinic (Norton Outreach)</t>
-  </si>
-  <si>
     <t>marondera</t>
   </si>
   <si>
-    <t>9. Marondera- Marondera District Hospital</t>
-  </si>
-  <si>
     <t>mahusekwa</t>
   </si>
   <si>
-    <t xml:space="preserve">10. Marondera- Mahusekwa Hospital
-</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
-    <t>11. Other</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -540,6 +515,72 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>3. City Med hospital</t>
+  </si>
+  <si>
+    <t>4. Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>5. Chitungwiza Central Hospital</t>
+  </si>
+  <si>
+    <t>7. Chegutu District Hospital</t>
+  </si>
+  <si>
+    <t>8. Monera clinic(Norton Outreach)</t>
+  </si>
+  <si>
+    <t>9. Marondera District Hospital</t>
+  </si>
+  <si>
+    <t>10. Mahusekwa Hospital</t>
+  </si>
+  <si>
+    <t>makumbe</t>
+  </si>
+  <si>
+    <t>11. Goromonzi-Makumbe Mission Hospital</t>
+  </si>
+  <si>
+    <t>ruwa</t>
+  </si>
+  <si>
+    <t>12. Goromonzi-Ruwa Rehab Hospital</t>
+  </si>
+  <si>
+    <t>kadoma</t>
+  </si>
+  <si>
+    <t>13. Sanyati-Kadoma Hospital</t>
+  </si>
+  <si>
+    <t>ndanga</t>
+  </si>
+  <si>
+    <t>14. Zaka-Ndanga District Hospital</t>
+  </si>
+  <si>
+    <t>musiso</t>
+  </si>
+  <si>
+    <t>15. Zaka-Musiso Mission Hospital</t>
+  </si>
+  <si>
+    <t>16. Mberengwa-Musiso Mission Hospital</t>
+  </si>
+  <si>
+    <t>17. Mberengwa-Mnene Mission Hospital</t>
+  </si>
+  <si>
+    <t>18. Mberengwa-Musume Mission Hospital</t>
+  </si>
+  <si>
+    <t>19. Mberengwa-Mberengwa District Hospital</t>
+  </si>
+  <si>
+    <t>20. Other</t>
   </si>
 </sst>
 </file>
@@ -559,44 +600,53 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF843C0B"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF548135"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -607,6 +657,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -625,6 +676,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -681,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -744,7 +796,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -972,25 +1023,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="44.5" customWidth="1"/>
-    <col min="4" max="4" width="37.25" customWidth="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="52.375" customWidth="1"/>
+    <col min="7" max="7" width="52.33203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
     <col min="9" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
+    <row r="1" spans="1:26" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1091,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75">
+    <row r="2" spans="1:26" ht="16">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1063,7 +1114,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75">
+    <row r="3" spans="1:26" ht="16">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1086,7 +1137,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75">
+    <row r="4" spans="1:26" ht="16">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1158,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75">
+    <row r="5" spans="1:26" ht="16">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1179,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75">
+    <row r="6" spans="1:26" ht="16">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -1149,7 +1200,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75">
+    <row r="7" spans="1:26" ht="16">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1219,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75">
+    <row r="8" spans="1:26" ht="16">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1193,7 +1244,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75">
+    <row r="9" spans="1:26" ht="16">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1214,7 +1265,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75">
+    <row r="10" spans="1:26" ht="16">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1235,7 +1286,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75">
+    <row r="11" spans="1:26" ht="16">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1250,7 +1301,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75">
+    <row r="12" spans="1:26" ht="16">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1265,7 +1316,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75">
+    <row r="13" spans="1:26" ht="16">
       <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
@@ -1301,7 +1352,7 @@
       <c r="Y13" s="14"/>
       <c r="Z13" s="14"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75">
+    <row r="14" spans="1:26" ht="16">
       <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
@@ -1339,7 +1390,7 @@
       <c r="Y14" s="14"/>
       <c r="Z14" s="14"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75">
+    <row r="15" spans="1:26" ht="16">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1375,7 +1426,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75">
+    <row r="16" spans="1:26" ht="16">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1409,7 +1460,7 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75">
+    <row r="17" spans="1:26" ht="16">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1443,7 +1494,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75">
+    <row r="18" spans="1:26" ht="16">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
@@ -1479,7 +1530,7 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75">
+    <row r="19" spans="1:26" ht="16">
       <c r="A19" s="8" t="s">
         <v>53</v>
       </c>
@@ -1515,7 +1566,7 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75">
+    <row r="20" spans="1:26" ht="16">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -1551,7 +1602,7 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75">
+    <row r="21" spans="1:26" ht="16">
       <c r="A21" s="12" t="s">
         <v>58</v>
       </c>
@@ -1587,7 +1638,7 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75">
+    <row r="22" spans="1:26" ht="16">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -1629,7 +1680,7 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75">
+    <row r="23" spans="1:26" ht="16">
       <c r="A23" s="8" t="s">
         <v>67</v>
       </c>
@@ -1669,7 +1720,7 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75">
+    <row r="24" spans="1:26" ht="16">
       <c r="A24" s="8" t="s">
         <v>53</v>
       </c>
@@ -1705,7 +1756,7 @@
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75">
+    <row r="25" spans="1:26" ht="16">
       <c r="A25" s="8" t="s">
         <v>74</v>
       </c>
@@ -1743,7 +1794,7 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75">
+    <row r="26" spans="1:26" ht="16">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -1787,7 +1838,7 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75">
+    <row r="27" spans="1:26" ht="16">
       <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
@@ -1817,7 +1868,7 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75">
+    <row r="28" spans="1:26" ht="16">
       <c r="A28" s="13" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1904,7 @@
       <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75">
+    <row r="29" spans="1:26" ht="16">
       <c r="A29" s="12" t="s">
         <v>85</v>
       </c>
@@ -1889,7 +1940,7 @@
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75">
+    <row r="30" spans="1:26" ht="16">
       <c r="A30" s="12" t="s">
         <v>39</v>
       </c>
@@ -1927,7 +1978,7 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75">
+    <row r="31" spans="1:26" ht="16">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
@@ -1993,7 +2044,7 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75">
+    <row r="33" spans="1:26" ht="16">
       <c r="A33" s="8" t="s">
         <v>53</v>
       </c>
@@ -2031,7 +2082,7 @@
       <c r="Y33" s="8"/>
       <c r="Z33" s="8"/>
     </row>
-    <row r="34" spans="1:26" ht="15.75">
+    <row r="34" spans="1:26" ht="16">
       <c r="A34" s="8" t="s">
         <v>96</v>
       </c>
@@ -2067,7 +2118,7 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75">
+    <row r="35" spans="1:26" ht="16">
       <c r="A35" s="12" t="s">
         <v>39</v>
       </c>
@@ -2103,7 +2154,7 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75">
+    <row r="36" spans="1:26" ht="16">
       <c r="A36" s="8" t="s">
         <v>53</v>
       </c>
@@ -2141,7 +2192,7 @@
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75">
+    <row r="37" spans="1:26" ht="16">
       <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
@@ -2179,7 +2230,7 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75">
+    <row r="38" spans="1:26" ht="16">
       <c r="A38" s="8" t="s">
         <v>105</v>
       </c>
@@ -2223,7 +2274,7 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75">
+    <row r="39" spans="1:26" ht="16">
       <c r="A39" s="13" t="s">
         <v>38</v>
       </c>
@@ -3328,21 +3379,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="31.25" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -3353,7 +3404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -3364,7 +3415,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -3375,17 +3426,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
         <v>117</v>
       </c>
@@ -3396,7 +3447,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
         <v>117</v>
       </c>
@@ -3407,7 +3458,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="16">
       <c r="A8" s="1" t="s">
         <v>117</v>
       </c>
@@ -3418,12 +3469,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
         <v>124</v>
       </c>
@@ -3434,7 +3485,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:3" ht="16">
       <c r="A11" s="1" t="s">
         <v>124</v>
       </c>
@@ -3484,159 +3535,237 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="28" t="s">
+      <c r="C20" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C21" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="28" t="s">
+      <c r="C22" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="29" t="s">
+      <c r="B23" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="28" t="s">
+      <c r="C23" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B24" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C24" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="28" t="s">
+      <c r="C25" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B26" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C26" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16">
+      <c r="A29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16">
+      <c r="A30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A36" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="28" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:3" ht="15.75">
-      <c r="A29" s="12"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="12"/>
-    </row>
-    <row r="30" spans="1:3" ht="15.75">
-      <c r="A30" s="12"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="27"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+      <c r="C36" s="28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="38" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -4594,105 +4723,105 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.875" customWidth="1"/>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="15" width="11.5" customWidth="1"/>
-    <col min="16" max="26" width="8.75" customWidth="1"/>
+    <col min="16" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B2" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C2" s="33">
+        <v>43894</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E2" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="H2" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="34">
-        <v>43894</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
user original name for former locations
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CB4B1F-45F9-BD44-9A44-4620284A7BD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8376FA92-0040-D94E-BAEC-58F1888F83B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,27 +517,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>3. City Med hospital</t>
-  </si>
-  <si>
-    <t>4. Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>5. Chitungwiza Central Hospital</t>
-  </si>
-  <si>
-    <t>7. Chegutu District Hospital</t>
-  </si>
-  <si>
-    <t>8. Monera clinic(Norton Outreach)</t>
-  </si>
-  <si>
-    <t>9. Marondera District Hospital</t>
-  </si>
-  <si>
-    <t>10. Mahusekwa Hospital</t>
-  </si>
-  <si>
     <t>makumbe</t>
   </si>
   <si>
@@ -581,6 +560,27 @@
   </si>
   <si>
     <t>20. Other</t>
+  </si>
+  <si>
+    <t>3. Chitungwiza-City Med hospital</t>
+  </si>
+  <si>
+    <t>4.  Chitungwiza-Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>5.  Chitungwiza-Chitungwiza Central Hospital</t>
+  </si>
+  <si>
+    <t>7. Chegutu- District Hospital</t>
+  </si>
+  <si>
+    <t>8. Chegutu-Monera clinic(Norton Outreach)</t>
+  </si>
+  <si>
+    <t>9. Marondera- Marondera District Hospital</t>
+  </si>
+  <si>
+    <t>10. Marondera- Mahusekwa Hospital</t>
   </si>
 </sst>
 </file>
@@ -3381,7 +3381,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3564,7 +3564,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -3575,7 +3575,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
@@ -3586,7 +3586,7 @@
         <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -3608,7 +3608,7 @@
         <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
@@ -3619,7 +3619,7 @@
         <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
@@ -3630,7 +3630,7 @@
         <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
@@ -3641,7 +3641,7 @@
         <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -3649,10 +3649,10 @@
         <v>133</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
@@ -3660,10 +3660,10 @@
         <v>133</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
@@ -3671,10 +3671,10 @@
         <v>133</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16">
@@ -3682,10 +3682,10 @@
         <v>133</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
@@ -3693,10 +3693,10 @@
         <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
@@ -3704,10 +3704,10 @@
         <v>133</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
@@ -3715,10 +3715,10 @@
         <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
@@ -3726,10 +3726,10 @@
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
@@ -3737,10 +3737,10 @@
         <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
@@ -3751,7 +3751,7 @@
         <v>147</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
ensure name matches the requirement doc
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8376FA92-0040-D94E-BAEC-58F1888F83B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2304DA09-D1A3-5F42-800A-06989597042D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="188">
   <si>
     <t>type</t>
   </si>
@@ -547,18 +547,6 @@
     <t>15. Zaka-Musiso Mission Hospital</t>
   </si>
   <si>
-    <t>16. Mberengwa-Musiso Mission Hospital</t>
-  </si>
-  <si>
-    <t>17. Mberengwa-Mnene Mission Hospital</t>
-  </si>
-  <si>
-    <t>18. Mberengwa-Musume Mission Hospital</t>
-  </si>
-  <si>
-    <t>19. Mberengwa-Mberengwa District Hospital</t>
-  </si>
-  <si>
     <t>20. Other</t>
   </si>
   <si>
@@ -581,6 +569,30 @@
   </si>
   <si>
     <t>10. Marondera- Mahusekwa Hospital</t>
+  </si>
+  <si>
+    <t>mnene</t>
+  </si>
+  <si>
+    <t>musume</t>
+  </si>
+  <si>
+    <t>mberengwa</t>
+  </si>
+  <si>
+    <t>masase</t>
+  </si>
+  <si>
+    <t>16. Mberengwa-Mnene Mission Hospital</t>
+  </si>
+  <si>
+    <t>17. Mberengwa-Musume Mission Hospital</t>
+  </si>
+  <si>
+    <t>18. Mberengwa-Mberengwa District Hospital</t>
+  </si>
+  <si>
+    <t>19. Masase Mission Hospital</t>
   </si>
 </sst>
 </file>
@@ -796,7 +808,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -806,6 +817,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3381,7 +3393,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3564,7 +3576,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -3575,7 +3587,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
@@ -3586,7 +3598,7 @@
         <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -3608,7 +3620,7 @@
         <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
@@ -3619,7 +3631,7 @@
         <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
@@ -3630,7 +3642,7 @@
         <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
@@ -3641,7 +3653,7 @@
         <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -3704,10 +3716,10 @@
         <v>133</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
@@ -3715,10 +3727,10 @@
         <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
@@ -3726,10 +3738,10 @@
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
@@ -3737,21 +3749,21 @@
         <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>176</v>
+      <c r="C36" s="33" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1"/>
@@ -4734,94 +4746,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="32">
         <v>43894</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
remove uneccesaru space from xlsx file
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2304DA09-D1A3-5F42-800A-06989597042D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F61089-1A57-8C4F-88E4-DF2E2339F84B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,12 +553,6 @@
     <t>3. Chitungwiza-City Med hospital</t>
   </si>
   <si>
-    <t>4.  Chitungwiza-Zengeza Clinic</t>
-  </si>
-  <si>
-    <t>5.  Chitungwiza-Chitungwiza Central Hospital</t>
-  </si>
-  <si>
     <t>7. Chegutu- District Hospital</t>
   </si>
   <si>
@@ -593,6 +587,12 @@
   </si>
   <si>
     <t>19. Masase Mission Hospital</t>
+  </si>
+  <si>
+    <t>4. Chitungwiza-Zengeza Clinic</t>
+  </si>
+  <si>
+    <t>5. Chitungwiza-Chitungwiza Central Hospital</t>
   </si>
 </sst>
 </file>
@@ -3393,7 +3393,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3587,7 +3587,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
@@ -3598,7 +3598,7 @@
         <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -3620,7 +3620,7 @@
         <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
@@ -3631,7 +3631,7 @@
         <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
@@ -3642,7 +3642,7 @@
         <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
@@ -3653,7 +3653,7 @@
         <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -3716,10 +3716,10 @@
         <v>133</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
@@ -3727,10 +3727,10 @@
         <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
@@ -3738,10 +3738,10 @@
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
@@ -3749,10 +3749,10 @@
         <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
117 add more site (#129)
* added missed site
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuel-amodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF8E1EA-1717-AA47-8D2B-BC348791577A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B73F660-76D6-4C4B-BB90-304F7C6DA7E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="191">
   <si>
     <t>type</t>
   </si>
@@ -538,18 +538,9 @@
     <t>ndanga</t>
   </si>
   <si>
-    <t>14. Zaka-Ndanga District Hospital</t>
-  </si>
-  <si>
     <t>musiso</t>
   </si>
   <si>
-    <t>15. Zaka-Musiso Mission Hospital</t>
-  </si>
-  <si>
-    <t>20. Other</t>
-  </si>
-  <si>
     <t>3. Chitungwiza-City Med hospital</t>
   </si>
   <si>
@@ -577,18 +568,6 @@
     <t>masase</t>
   </si>
   <si>
-    <t>16. Mberengwa-Mnene Mission Hospital</t>
-  </si>
-  <si>
-    <t>17. Mberengwa-Musume Mission Hospital</t>
-  </si>
-  <si>
-    <t>18. Mberengwa-Mberengwa District Hospital</t>
-  </si>
-  <si>
-    <t>19. Masase Mission Hospital</t>
-  </si>
-  <si>
     <t>4. Chitungwiza-Zengeza Clinic</t>
   </si>
   <si>
@@ -596,6 +575,33 @@
   </si>
   <si>
     <t>minimal</t>
+  </si>
+  <si>
+    <t>kadoma_city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. Sanyati-Kadoma City </t>
+  </si>
+  <si>
+    <t>15. Zaka-Ndanga District Hospital</t>
+  </si>
+  <si>
+    <t>16. Zaka-Musiso Mission Hospital</t>
+  </si>
+  <si>
+    <t>17. Mberengwa-Mnene Mission Hospital</t>
+  </si>
+  <si>
+    <t>18. Mberengwa-Musume Mission Hospital</t>
+  </si>
+  <si>
+    <t>19. Mberengwa-Mberengwa District Hospital</t>
+  </si>
+  <si>
+    <t>21. Other</t>
+  </si>
+  <si>
+    <t>20. Mberengwa-Masase Mission Hospital</t>
   </si>
 </sst>
 </file>
@@ -748,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -821,6 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
@@ -1629,7 +1636,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>33</v>
@@ -3394,11 +3401,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C993"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3581,7 +3588,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -3592,7 +3599,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
@@ -3603,7 +3610,7 @@
         <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -3625,7 +3632,7 @@
         <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
@@ -3636,7 +3643,7 @@
         <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
@@ -3647,7 +3654,7 @@
         <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
@@ -3658,7 +3665,7 @@
         <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -3699,10 +3706,10 @@
         <v>133</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
@@ -3710,10 +3717,10 @@
         <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
@@ -3721,68 +3728,100 @@
         <v>133</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="33" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="33" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="38" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1"/>
+      <c r="C37" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
+      <c r="S37" s="33"/>
+      <c r="T37" s="33"/>
+      <c r="U37" s="33"/>
+      <c r="V37" s="33"/>
+      <c r="W37" s="33"/>
+      <c r="X37" s="33"/>
+      <c r="Y37" s="33"/>
+      <c r="Z37" s="33"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
change from select-one to db-object (#263)
* change from select-one to db-object

* fix test

* make group and add name

* fix test

* fix name issue

* group label re name

Co-authored-by: Emmanuel Amodu <emmanuelamodu@Emmanuels-MacBook-Pro-2.local>
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/client_review.xlsx
+++ b/zazic-scale-up/forms/app/client_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC8C41E-358A-034E-927E-0FD53106A82C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC02BB-13B5-CC47-8747-E8A0F52E2519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="232">
   <si>
     <t>type</t>
   </si>
@@ -203,12 +203,6 @@
     <t>${client_came} = 'yes'</t>
   </si>
   <si>
-    <t>select_one facilities</t>
-  </si>
-  <si>
-    <t>clinic_name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Which clinic? </t>
   </si>
   <si>
@@ -216,18 +210,6 @@
   </si>
   <si>
     <t>Please type in name characters e.g letters and space.</t>
-  </si>
-  <si>
-    <t>clinic_name_other</t>
-  </si>
-  <si>
-    <t>Specify Other</t>
-  </si>
-  <si>
-    <t>${clinic_name} = 'other'</t>
-  </si>
-  <si>
-    <t>Please enter a valid clinic name</t>
   </si>
   <si>
     <t>date</t>
@@ -478,9 +460,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>minimal</t>
-  </si>
-  <si>
     <t>guruve_hospital</t>
   </si>
   <si>
@@ -740,6 +719,12 @@
   </si>
   <si>
     <t>44. Other</t>
+  </si>
+  <si>
+    <t>db:health_center</t>
+  </si>
+  <si>
+    <t>health_center</t>
   </si>
 </sst>
 </file>
@@ -749,7 +734,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -837,6 +822,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -892,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -966,6 +958,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,11 +1174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1763,24 +1756,20 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="16">
-      <c r="A21" s="12" t="s">
-        <v>58</v>
+      <c r="A21" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>60</v>
+        <v>231</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1802,27 +1791,23 @@
     </row>
     <row r="22" spans="1:26" ht="16">
       <c r="A22" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>66</v>
-      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1843,26 +1828,20 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="16">
-      <c r="A23" s="8" t="s">
-        <v>67</v>
+      <c r="A23" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>71</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1883,20 +1862,14 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="16">
-      <c r="A24" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>73</v>
-      </c>
+      <c r="A24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -1920,23 +1893,25 @@
     </row>
     <row r="25" spans="1:26" ht="16">
       <c r="A25" s="8" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1957,31 +1932,23 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="16">
-      <c r="A26" s="12" t="s">
-        <v>16</v>
+      <c r="A26" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -2001,14 +1968,22 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="16">
-      <c r="A27" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -2031,23 +2006,31 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="16">
-      <c r="A28" s="13" t="s">
-        <v>11</v>
+      <c r="A28" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>52</v>
+        <v>72</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="F28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -2067,20 +2050,14 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="16">
-      <c r="A29" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>87</v>
-      </c>
+      <c r="A29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
@@ -2103,27 +2080,25 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="16">
-      <c r="A30" s="12" t="s">
-        <v>39</v>
+      <c r="A30" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="12" t="s">
-        <v>89</v>
-      </c>
+      <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
@@ -2142,19 +2117,17 @@
     </row>
     <row r="31" spans="1:26" ht="16">
       <c r="A31" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>92</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="12" t="s">
         <v>33</v>
       </c>
       <c r="G31" s="8"/>
@@ -2178,18 +2151,28 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="16"/>
+    <row r="32" spans="1:26" ht="16">
+      <c r="A32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="12"/>
+      <c r="F32" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
+      <c r="K32" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -2207,17 +2190,17 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="16">
-      <c r="A33" s="8" t="s">
-        <v>53</v>
+      <c r="A33" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
@@ -2244,24 +2227,16 @@
       <c r="Y33" s="8"/>
       <c r="Z33" s="8"/>
     </row>
-    <row r="34" spans="1:26" ht="16">
-      <c r="A34" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>99</v>
-      </c>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="F34" s="12"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="12"/>
+      <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -2281,25 +2256,27 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="16">
-      <c r="A35" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="8"/>
+      <c r="A35" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="F35" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
-      <c r="K35" s="12" t="s">
-        <v>101</v>
-      </c>
+      <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -2318,24 +2295,22 @@
     </row>
     <row r="36" spans="1:26" ht="16">
       <c r="A36" s="8" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
@@ -2355,27 +2330,25 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="16">
-      <c r="A37" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>104</v>
-      </c>
+      <c r="A37" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
+      <c r="K37" s="12" t="s">
+        <v>95</v>
+      </c>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -2394,30 +2367,24 @@
     </row>
     <row r="38" spans="1:26" ht="16">
       <c r="A38" s="8" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>104</v>
+        <v>66</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>82</v>
-      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -2437,14 +2404,22 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" ht="16">
-      <c r="A39" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="8"/>
+      <c r="A39" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="F39" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
@@ -2466,24 +2441,32 @@
       <c r="Y39" s="8"/>
       <c r="Z39" s="8"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1">
+    <row r="40" spans="1:26" ht="16">
       <c r="A40" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -2502,27 +2485,17 @@
       <c r="Y40" s="8"/>
       <c r="Z40" s="8"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>110</v>
-      </c>
+    <row r="41" spans="1:26" ht="16">
+      <c r="A41" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2543,22 +2516,96 @@
       <c r="Z41" s="8"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+      <c r="Z42" s="8"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+      <c r="Z43" s="8"/>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="46" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="47" spans="1:26" ht="15.75" customHeight="1"/>
@@ -3531,6 +3578,8 @@
     <row r="1014" ht="15.75" customHeight="1"/>
     <row r="1015" ht="15.75" customHeight="1"/>
     <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -3541,9 +3590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3557,7 +3606,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3568,24 +3617,24 @@
     </row>
     <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
@@ -3600,35 +3649,35 @@
     </row>
     <row r="6" spans="1:3" ht="16">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
       <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -3638,57 +3687,57 @@
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
       <c r="A11" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
@@ -3698,233 +3747,233 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
       <c r="A29" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16">
       <c r="A30" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:26" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
@@ -3951,275 +4000,275 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D40" s="34"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D41" s="34"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D42" s="34"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D43" s="34"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D44" s="34"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D45" s="34"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D46" s="34"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D47" s="34"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D48" s="34"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D49" s="34"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D50" s="34"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D51" s="34"/>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D52" s="34"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D53" s="34"/>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D54" s="34"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D55" s="34"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D56" s="34"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D57" s="34"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D58" s="34"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D59" s="34"/>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
       <c r="A60" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B60" s="33" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1"/>
@@ -5178,31 +5227,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
@@ -5224,29 +5273,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C2" s="32">
         <v>43894</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="31" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>

</xml_diff>